<commit_message>
updated xlsx file and csv function
</commit_message>
<xml_diff>
--- a/week-ending-2020-10-24.xlsx
+++ b/week-ending-2020-10-24.xlsx
@@ -953,7 +953,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1003,6 +1003,50 @@
         <v>33</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1010,7 +1054,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1072,6 +1116,62 @@
         <v>33</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1079,7 +1179,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1139,6 +1239,62 @@
       </c>
       <c r="D4" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scraping all data for first 6 available week
</commit_message>
<xml_diff>
--- a/week-ending-2020-10-24.xlsx
+++ b/week-ending-2020-10-24.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="199">
   <si>
     <t>(n)</t>
   </si>
@@ -33,372 +33,513 @@
     <t>Percent</t>
   </si>
   <si>
+    <t>southeast</t>
+  </si>
+  <si>
     <t>northeast</t>
   </si>
   <si>
-    <t>southeast</t>
+    <t>central</t>
+  </si>
+  <si>
+    <t>metro_south</t>
   </si>
   <si>
     <t>eastern</t>
   </si>
   <si>
-    <t>central</t>
-  </si>
-  <si>
-    <t>metro_south</t>
-  </si>
-  <si>
     <t>western</t>
   </si>
   <si>
-    <t>somerville district</t>
-  </si>
-  <si>
-    <t>taunton district</t>
+    <t>malden district</t>
+  </si>
+  <si>
+    <t>pittsfield district</t>
+  </si>
+  <si>
+    <t>natick district</t>
+  </si>
+  <si>
+    <t>bmc east boston</t>
+  </si>
+  <si>
+    <t>barnstable district</t>
+  </si>
+  <si>
+    <t>lynn district</t>
+  </si>
+  <si>
+    <t>eastern hampshire district</t>
+  </si>
+  <si>
+    <t>plymouth district</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>21.1%</t>
+  </si>
+  <si>
+    <t>20.0%</t>
+  </si>
+  <si>
+    <t>17.9%</t>
+  </si>
+  <si>
+    <t>11.6%</t>
+  </si>
+  <si>
+    <t>9.5%</t>
+  </si>
+  <si>
+    <t>5.3%</t>
+  </si>
+  <si>
+    <t>3.2%</t>
+  </si>
+  <si>
+    <t>2.1%</t>
+  </si>
+  <si>
+    <t>1.1%</t>
+  </si>
+  <si>
+    <t>Plaintiffs</t>
+  </si>
+  <si>
+    <t>Defendants</t>
+  </si>
+  <si>
+    <t>Corporate Entity</t>
+  </si>
+  <si>
+    <t>Natural Person</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>(%)</t>
+  </si>
+  <si>
+    <t>34.7%</t>
+  </si>
+  <si>
+    <t>65.3%</t>
+  </si>
+  <si>
+    <t>100.0%</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>Has Attorney</t>
+  </si>
+  <si>
+    <t>Pro Se</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>33.7%</t>
+  </si>
+  <si>
+    <t>27.4%</t>
+  </si>
+  <si>
+    <t>61.1%</t>
+  </si>
+  <si>
+    <t>37.9%</t>
+  </si>
+  <si>
+    <t>38.9%</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>90.5%</t>
+  </si>
+  <si>
+    <t>Number of Adults in Households</t>
+  </si>
+  <si>
+    <t>Note: Households may appear with zero adults either in cases of identity protection (e.g., 42 USC Sections 13701 through 1404 Violence Against Women Act) or where no adult (18 or over) remains in the home.</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7.4%</t>
+  </si>
+  <si>
+    <t>54.7%</t>
+  </si>
+  <si>
+    <t>28.4%</t>
+  </si>
+  <si>
+    <t>8.4%</t>
+  </si>
+  <si>
+    <t>Initiating Action</t>
+  </si>
+  <si>
+    <t>Non-payment</t>
+  </si>
+  <si>
+    <t>Cause</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>No Fault</t>
+  </si>
+  <si>
+    <t>Foreclosure</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>35.8%</t>
+  </si>
+  <si>
+    <t>31.6%</t>
+  </si>
+  <si>
+    <t>14.7%</t>
+  </si>
+  <si>
+    <t>13.7%</t>
+  </si>
+  <si>
+    <t>4.2%</t>
+  </si>
+  <si>
+    <t>Municipality</t>
+  </si>
+  <si>
+    <t>Residents</t>
+  </si>
+  <si>
+    <t>Baldwinville</t>
+  </si>
+  <si>
+    <t>Sherborn</t>
+  </si>
+  <si>
+    <t>Provincetown</t>
+  </si>
+  <si>
+    <t>Eastham</t>
+  </si>
+  <si>
+    <t>Yarmouth Port</t>
+  </si>
+  <si>
+    <t>Dover</t>
+  </si>
+  <si>
+    <t>East Falmouth</t>
+  </si>
+  <si>
+    <t>Whitinsville</t>
+  </si>
+  <si>
+    <t>Upton</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Cherry Valley</t>
+  </si>
+  <si>
+    <t>Hull</t>
+  </si>
+  <si>
+    <t>Athol</t>
+  </si>
+  <si>
+    <t>Dudley</t>
+  </si>
+  <si>
+    <t>Everett</t>
+  </si>
+  <si>
+    <t>Hyannis</t>
+  </si>
+  <si>
+    <t>Northborough</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>Belchertown</t>
+  </si>
+  <si>
+    <t>East Longmeadow</t>
+  </si>
+  <si>
+    <t>Fairhaven</t>
+  </si>
+  <si>
+    <t>New Bedford</t>
+  </si>
+  <si>
+    <t>Brockton</t>
+  </si>
+  <si>
+    <t>Foxborough</t>
+  </si>
+  <si>
+    <t>Marblehead</t>
+  </si>
+  <si>
+    <t>Southbridge</t>
+  </si>
+  <si>
+    <t>Webster</t>
+  </si>
+  <si>
+    <t>Barnstable</t>
+  </si>
+  <si>
+    <t>Dorchester</t>
+  </si>
+  <si>
+    <t>E. Boston</t>
+  </si>
+  <si>
+    <t>Middleborough</t>
+  </si>
+  <si>
+    <t>Pittsfield</t>
+  </si>
+  <si>
+    <t>Stoneham</t>
+  </si>
+  <si>
+    <t>Winchester</t>
+  </si>
+  <si>
+    <t>Agawam</t>
+  </si>
+  <si>
+    <t>Bridgewater</t>
+  </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>Haverhill</t>
+  </si>
+  <si>
+    <t>Lexington</t>
+  </si>
+  <si>
+    <t>Malden</t>
+  </si>
+  <si>
+    <t>Norwood</t>
+  </si>
+  <si>
+    <t>Plymouth</t>
+  </si>
+  <si>
+    <t>Randolph</t>
+  </si>
+  <si>
+    <t>Roslindale</t>
+  </si>
+  <si>
+    <t>Tewksbury</t>
+  </si>
+  <si>
+    <t>Worcester</t>
+  </si>
+  <si>
+    <t>Beverly</t>
+  </si>
+  <si>
+    <t>Billerica</t>
+  </si>
+  <si>
+    <t>Fall River</t>
+  </si>
+  <si>
+    <t>Lawrence</t>
+  </si>
+  <si>
+    <t>Leominster</t>
+  </si>
+  <si>
+    <t>Lowell</t>
+  </si>
+  <si>
+    <t>Lynn</t>
+  </si>
+  <si>
+    <t>Taunton</t>
+  </si>
+  <si>
+    <t>(not given)</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Cambridge</t>
+  </si>
+  <si>
+    <t>Springfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate per 100,000 residents based on 2010 census. Municipalities do not appear if no evictions filed. Where neighborhoods are commonly recognized as municipalities, data appears under the neighborhood rather than the legal entity (e.g., "Roxbury" is separate from "Boston".) Where municipalities have alternate spellings (e.g., Marlboro for Marlborough), totals appear under the long form. Efforts are made to correct clerical errors in the court database, but clerical errors may appear. </t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Renter Households</t>
+  </si>
+  <si>
+    <t>Berkshire</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>Essex</t>
+  </si>
+  <si>
+    <t>Middlesex</t>
+  </si>
+  <si>
+    <t>Hampshire</t>
+  </si>
+  <si>
+    <t>Norfolk</t>
+  </si>
+  <si>
+    <t>Hampden</t>
+  </si>
+  <si>
+    <t>Suffolk</t>
+  </si>
+  <si>
+    <t>Dukes</t>
+  </si>
+  <si>
+    <t>Nantucket</t>
+  </si>
+  <si>
+    <t>Rate per 100,000 renter households based on 2019 ACS. Counties appear even if no evictions filed.</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>32.7%</t>
-  </si>
-  <si>
-    <t>16.3%</t>
-  </si>
-  <si>
-    <t>12.2%</t>
-  </si>
-  <si>
-    <t>10.2%</t>
-  </si>
-  <si>
-    <t>2.0%</t>
-  </si>
-  <si>
-    <t>Plaintiffs</t>
-  </si>
-  <si>
-    <t>Defendants</t>
-  </si>
-  <si>
-    <t>Corporate Entity</t>
-  </si>
-  <si>
-    <t>Natural Person</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>(%)</t>
-  </si>
-  <si>
-    <t>34.7%</t>
-  </si>
-  <si>
-    <t>65.3%</t>
-  </si>
-  <si>
-    <t>100.0%</t>
-  </si>
-  <si>
-    <t>0.0%</t>
-  </si>
-  <si>
-    <t>Has Attorney</t>
-  </si>
-  <si>
-    <t>Pro Se</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>24.5%</t>
-  </si>
-  <si>
-    <t>57.1%</t>
-  </si>
-  <si>
-    <t>40.8%</t>
-  </si>
-  <si>
-    <t>42.9%</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>89.8%</t>
-  </si>
-  <si>
-    <t>Number of Adults in Households</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>73.5%</t>
-  </si>
-  <si>
-    <t>20.4%</t>
-  </si>
-  <si>
-    <t>6.1%</t>
-  </si>
-  <si>
-    <t>Initiating Action</t>
-  </si>
-  <si>
-    <t>Cause</t>
-  </si>
-  <si>
-    <t>Non-payment</t>
-  </si>
-  <si>
-    <t>No Fault</t>
-  </si>
-  <si>
-    <t>Foreclosure</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>36.7%</t>
-  </si>
-  <si>
-    <t>4.1%</t>
-  </si>
-  <si>
-    <t>Municipality</t>
-  </si>
-  <si>
-    <t>Residents</t>
-  </si>
-  <si>
-    <t>Vineyard Haven</t>
-  </si>
-  <si>
-    <t>Osterville</t>
-  </si>
-  <si>
-    <t>East Falmouth</t>
-  </si>
-  <si>
-    <t>Topsfield</t>
-  </si>
-  <si>
-    <t>Shirley</t>
-  </si>
-  <si>
-    <t>Southbridge</t>
-  </si>
-  <si>
-    <t>Amesbury</t>
-  </si>
-  <si>
-    <t>Brockton</t>
-  </si>
-  <si>
-    <t>Newburyport</t>
-  </si>
-  <si>
-    <t>Pembroke</t>
-  </si>
-  <si>
-    <t>Hingham</t>
-  </si>
-  <si>
-    <t>Pittsfield</t>
-  </si>
-  <si>
-    <t>Bridgewater</t>
-  </si>
-  <si>
-    <t>Danvers</t>
-  </si>
-  <si>
-    <t>Haverhill</t>
-  </si>
-  <si>
-    <t>Lawrence</t>
-  </si>
-  <si>
-    <t>Marshfield</t>
-  </si>
-  <si>
-    <t>Natick</t>
-  </si>
-  <si>
-    <t>Beverly</t>
-  </si>
-  <si>
-    <t>Chelsea</t>
-  </si>
-  <si>
-    <t>Dorchester</t>
-  </si>
-  <si>
-    <t>Everett</t>
-  </si>
-  <si>
-    <t>Lynn</t>
-  </si>
-  <si>
-    <t>Methuen</t>
-  </si>
-  <si>
-    <t>New Bedford</t>
-  </si>
-  <si>
-    <t>Somerville</t>
-  </si>
-  <si>
-    <t>South Boston</t>
-  </si>
-  <si>
-    <t>Chicopee</t>
-  </si>
-  <si>
-    <t>Malden</t>
-  </si>
-  <si>
-    <t>Medford</t>
-  </si>
-  <si>
-    <t>Springfield</t>
-  </si>
-  <si>
-    <t>Worcester</t>
-  </si>
-  <si>
-    <t>(not given)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate per 100,000 residents based on 2010 census. Municipalities do not appear if no evictions filed. Where neighborhoods are commonly recognized as municipalities, data appears under the neighborhood rather than the legal entity (e.g., "Roxbury" is separate from "Boston".) Where municipalities have alternate spellings (e.g., Marlboro for Marlborough), totals appear under the long form. Efforts are made to correct clerical errors in the court database, but clerical errors may appear. </t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>County</t>
-  </si>
-  <si>
-    <t>Renter Households</t>
-  </si>
-  <si>
-    <t>Dukes</t>
-  </si>
-  <si>
-    <t>Plymouth</t>
-  </si>
-  <si>
-    <t>Berkshire</t>
-  </si>
-  <si>
-    <t>Essex</t>
-  </si>
-  <si>
-    <t>Barnstable</t>
-  </si>
-  <si>
-    <t>Hampden</t>
-  </si>
-  <si>
-    <t>Middlesex</t>
-  </si>
-  <si>
-    <t>Bristol</t>
-  </si>
-  <si>
-    <t>Suffolk</t>
-  </si>
-  <si>
-    <t>Franklin</t>
-  </si>
-  <si>
-    <t>Hampshire</t>
-  </si>
-  <si>
-    <t>Nantucket</t>
-  </si>
-  <si>
-    <t>Norfolk</t>
-  </si>
-  <si>
-    <t>Rate per 100,000 renter households based on 2019 ACS. Counties appear even if no evictions filed.</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>Households</t>
   </si>
   <si>
@@ -447,9 +588,6 @@
     <t>316,162</t>
   </si>
   <si>
-    <t>20.0%</t>
-  </si>
-  <si>
     <t>30.0%</t>
   </si>
   <si>
@@ -475,9 +613,6 @@
   </si>
   <si>
     <t>30.8%</t>
-  </si>
-  <si>
-    <t>31.6%</t>
   </si>
   <si>
     <t>63.7%</t>
@@ -841,7 +976,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -863,10 +998,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -874,10 +1009,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -885,10 +1020,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -896,10 +1031,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -907,10 +1042,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -918,10 +1053,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -929,10 +1064,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -940,10 +1075,76 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -961,46 +1162,46 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1008,43 +1209,43 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1062,58 +1263,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1121,55 +1322,55 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
         <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1187,58 +1388,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1246,55 +1447,55 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1505,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1312,7 +1513,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1323,46 +1524,73 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1380,7 +1608,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1391,57 +1619,57 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1679,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1459,10 +1687,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1470,370 +1698,645 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>126</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1851,10 +2354,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1862,161 +2365,161 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>164</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2034,167 +2537,167 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C15" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>